<commit_message>
Refactored how card effects are handled
</commit_message>
<xml_diff>
--- a/Assets/Dungeon Decks Design.xlsx
+++ b/Assets/Dungeon Decks Design.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Unity Projects\Dungeon Decks\Assets\ScriptableObjects\Databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\Dungeon Decks\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25455F7-4052-4C8C-A77D-65B2C4BDFD56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
@@ -17,22 +18,30 @@
     <sheet name="Classes" sheetId="3" r:id="rId3"/>
     <sheet name="Cards" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Zachary Waller</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -152,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -176,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0">
+    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -200,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -224,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0">
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -248,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0">
+    <comment ref="E29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -272,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E16" authorId="0" shapeId="0">
+    <comment ref="E33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -296,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0" shapeId="0">
+    <comment ref="E34" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -330,7 +339,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0">
+    <comment ref="E35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -359,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
   <si>
     <t>Bat</t>
   </si>
@@ -451,9 +460,6 @@
     <t>PowerLevel</t>
   </si>
   <si>
-    <t>Potions</t>
-  </si>
-  <si>
     <t>Relics</t>
   </si>
   <si>
@@ -496,30 +502,15 @@
     <t>Barbarian</t>
   </si>
   <si>
-    <t>Magus</t>
-  </si>
-  <si>
     <t>Paladin</t>
   </si>
   <si>
-    <t>Mage</t>
-  </si>
-  <si>
-    <t>Witch Hunter</t>
-  </si>
-  <si>
     <t>Hunter</t>
   </si>
   <si>
     <t>Nightblade</t>
   </si>
   <si>
-    <t>Monk</t>
-  </si>
-  <si>
-    <t>Shaman</t>
-  </si>
-  <si>
     <t>DR</t>
   </si>
   <si>
@@ -595,15 +586,9 @@
     <t>Roll</t>
   </si>
   <si>
-    <t>Cauterize</t>
-  </si>
-  <si>
     <t>Spears</t>
   </si>
   <si>
-    <t>Spec</t>
-  </si>
-  <si>
     <t>45/45/10% Primary/Secondary/Other Stat Relic</t>
   </si>
   <si>
@@ -622,18 +607,9 @@
     <t>Battle Mage</t>
   </si>
   <si>
-    <t>Priest</t>
-  </si>
-  <si>
     <t>Ranger</t>
   </si>
   <si>
-    <t>Cleric</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
     <t>Purify</t>
   </si>
   <si>
@@ -655,18 +631,12 @@
     <t>Leap 3 squares - Card</t>
   </si>
   <si>
-    <t>Take no damage for X turns - Card</t>
-  </si>
-  <si>
     <t>Adds all burns together and deals half of total outright and applies rest as burn - Card</t>
   </si>
   <si>
     <t>Staggers out all damage taken over 10 turns - Aura</t>
   </si>
   <si>
-    <t>Revive</t>
-  </si>
-  <si>
     <t>Heals for half of missing health - Card</t>
   </si>
   <si>
@@ -676,28 +646,64 @@
     <t>Quiver</t>
   </si>
   <si>
-    <t>Can use ranged attacks twice before discarding - Aura</t>
-  </si>
-  <si>
     <t>Salvage</t>
   </si>
   <si>
-    <t>Plus (1% max AP) AP when discarding - Aura</t>
-  </si>
-  <si>
     <t>Conduit</t>
   </si>
   <si>
-    <t>Plus (1% max HP) HP when discarding - Aura</t>
-  </si>
-  <si>
     <t>Armor cards  50% more effective - Aura</t>
+  </si>
+  <si>
+    <t>Ignite</t>
+  </si>
+  <si>
+    <t>Plus (1% max HP) HP when discarding - Aura (I don't like this)</t>
+  </si>
+  <si>
+    <t>Plus (1% max AP) AP when discarding - Aura (I don't like this)</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>Punch</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Bonus</t>
+  </si>
+  <si>
+    <t>Str 0.5 Dex 0.35</t>
+  </si>
+  <si>
+    <t>Consumables</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>Wizard</t>
+  </si>
+  <si>
+    <t>Lay on Hands</t>
+  </si>
+  <si>
+    <t>Enemies won't pursue you for 5 turns</t>
+  </si>
+  <si>
+    <t>Ignore the next source of damage - Card</t>
+  </si>
+  <si>
+    <t>Gain two ranged attack cards whenever you pick one up - Aura</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -897,14 +903,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="H9:I18" totalsRowShown="0">
-  <autoFilter ref="H9:I18"/>
-  <sortState ref="H10:I17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="H9:I19" totalsRowShown="0">
+  <autoFilter ref="H9:I19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H10:I17">
     <sortCondition ref="H9:H17"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Card"/>
-    <tableColumn id="2" name="Effect"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Card"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Effect"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1172,12 +1178,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,7 +1743,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G24">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G24">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1745,12 +1751,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,13 +1768,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1">
         <v>0.7</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1777,7 +1783,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="B2" s="1">
         <v>0.2</v>
@@ -1789,13 +1795,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -1811,7 +1817,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1">
         <f>SUM(B1:B3)</f>
@@ -1830,11 +1836,11 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
@@ -1848,13 +1854,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="D14" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1870,10 +1876,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -1888,10 +1894,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -1911,17 +1917,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" customWidth="1"/>
     <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="9" max="9" width="77.28515625" customWidth="1"/>
@@ -1930,480 +1937,457 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
         <v>41</v>
-      </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
       <c r="D3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>87</v>
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="I9" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="I10" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" t="s">
-        <v>108</v>
+        <v>76</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="H12" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="I12" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" t="s">
         <v>94</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H13" t="s">
-        <v>103</v>
-      </c>
-      <c r="I13" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="I14" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="H15" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" t="s">
-        <v>84</v>
-      </c>
-      <c r="H15" t="s">
-        <v>101</v>
-      </c>
       <c r="I15" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H16" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="I16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="I17" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
       <c r="H18" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="I18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="17"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="8"/>
+      <c r="C24" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="8"/>
+      <c r="C25" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="8"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A13:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="5" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="8"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="11"/>
+    <row r="13" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="13" t="s">
-        <v>70</v>
-      </c>
+    <row r="14" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="13" t="s">
-        <v>60</v>
-      </c>
+    <row r="15" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
       <c r="I21" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Slight redesign to the stat panel in in-game UI
</commit_message>
<xml_diff>
--- a/Assets/Dungeon Decks Design.xlsx
+++ b/Assets/Dungeon Decks Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\Dungeon Decks\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25455F7-4052-4C8C-A77D-65B2C4BDFD56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8F7874-A460-4F05-9938-C4895E380528}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21645" yWindow="3180" windowWidth="19575" windowHeight="10140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Enemies" sheetId="1" r:id="rId1"/>
@@ -368,7 +368,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
   <si>
     <t>Bat</t>
   </si>
@@ -698,6 +698,18 @@
   </si>
   <si>
     <t>Gain two ranged attack cards whenever you pick one up - Aura</t>
+  </si>
+  <si>
+    <t>Dispatch</t>
+  </si>
+  <si>
+    <t>Able to use melee attacks at a range for X turns</t>
+  </si>
+  <si>
+    <t>Spellstrikes</t>
+  </si>
+  <si>
+    <t>Also Punch when using a spell in melee</t>
   </si>
 </sst>
 </file>
@@ -903,8 +915,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="H9:I19" totalsRowShown="0">
-  <autoFilter ref="H9:I19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="H9:I21" totalsRowShown="0">
+  <autoFilter ref="H9:I21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H10:I17">
     <sortCondition ref="H9:H17"/>
   </sortState>
@@ -1182,7 +1194,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -1756,7 +1768,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,7 +1934,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,10 +2079,15 @@
       <c r="A13" t="s">
         <v>40</v>
       </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="H13" t="s">
         <v>90</v>
       </c>
@@ -2181,6 +2198,12 @@
       <c r="E20" s="16" t="s">
         <v>62</v>
       </c>
+      <c r="H20" t="s">
+        <v>110</v>
+      </c>
+      <c r="I20" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
@@ -2192,6 +2215,12 @@
       <c r="D21" s="11"/>
       <c r="E21" s="13" t="s">
         <v>69</v>
+      </c>
+      <c r="H21" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2340,7 +2369,7 @@
   <dimension ref="A13:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E18"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>